<commit_message>
thêm encrypt password + file excel chứa password sv
</commit_message>
<xml_diff>
--- a/thêm tài khoản sv.xlsx
+++ b/thêm tài khoản sv.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\OneDrive\Desktop\web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{1E81326D-B143-47E4-AF49-1302310900A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BD96F536-36A7-4465-A197-38AEDB1A2A1D}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{1E81326D-B143-47E4-AF49-1302310900A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D8D5E3BA-9DA5-4F59-800C-EE9291963555}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6482D4AB-D8AC-4714-ADF4-892F148B6002}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
   <si>
     <t>tên</t>
   </si>
@@ -45,26 +45,59 @@
     <t>mật khẩu</t>
   </si>
   <si>
+    <t>k62</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>abcde</t>
+  </si>
+  <si>
+    <t>thịnh</t>
+  </si>
+  <si>
     <t>nam</t>
   </si>
   <si>
-    <t>k62</t>
-  </si>
-  <si>
-    <t>abcd</t>
+    <t>cxzv</t>
   </si>
   <si>
     <t>linh</t>
   </si>
   <si>
-    <t>abcde</t>
+    <t>minh</t>
+  </si>
+  <si>
+    <t>hiếu</t>
+  </si>
+  <si>
+    <t>văn a</t>
+  </si>
+  <si>
+    <t>văn b</t>
+  </si>
+  <si>
+    <t>văn c</t>
+  </si>
+  <si>
+    <t>dương</t>
+  </si>
+  <si>
+    <t>dũng</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>none</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,6 +109,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -424,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68345002-079F-415D-BF39-89DF31C9ED0B}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -454,33 +493,174 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="2">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4" s="2">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="2">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="2">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="2">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2">
+        <v>20</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>